<commit_message>
fixed bug prev info creation; added plot functions
</commit_message>
<xml_diff>
--- a/exp_results.xlsx
+++ b/exp_results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="28620" windowHeight="12915" activeTab="5"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="28620" windowHeight="12915" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Direct" sheetId="1" r:id="rId1"/>
@@ -13,13 +13,14 @@
     <sheet name="Direct_withPrev" sheetId="4" r:id="rId4"/>
     <sheet name="LogTrainLogTest_withPrev" sheetId="5" r:id="rId5"/>
     <sheet name="logTrainDirectTest_withPrev" sheetId="6" r:id="rId6"/>
+    <sheet name="logTrainDirectTest_withPrev_FIX" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="43">
   <si>
     <t>adagio_cmp_1098432-512p</t>
   </si>
@@ -146,6 +147,9 @@
   <si>
     <t>prev_time_mpi</t>
   </si>
+  <si>
+    <t>adagio_nas_1098439.mg.E.128</t>
+  </si>
 </sst>
 </file>
 
@@ -188,7 +192,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -258,6 +262,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -429,7 +439,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="140">
+  <cellXfs count="141">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -606,6 +616,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -8148,7 +8159,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AO45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
@@ -13054,8 +13065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AO45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G65" sqref="G65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13078,6 +13089,19 @@
     <col min="17" max="18" width="10.85546875" customWidth="1"/>
     <col min="19" max="20" width="16.42578125" customWidth="1"/>
     <col min="21" max="21" width="17.5703125" customWidth="1"/>
+    <col min="26" max="26" width="10.5703125" customWidth="1"/>
+    <col min="27" max="27" width="12.42578125" customWidth="1"/>
+    <col min="28" max="28" width="11.140625" customWidth="1"/>
+    <col min="29" max="29" width="21.28515625" customWidth="1"/>
+    <col min="30" max="30" width="13.7109375" customWidth="1"/>
+    <col min="31" max="31" width="10.5703125" customWidth="1"/>
+    <col min="32" max="32" width="11" customWidth="1"/>
+    <col min="33" max="33" width="10.5703125" customWidth="1"/>
+    <col min="36" max="36" width="11.85546875" customWidth="1"/>
+    <col min="38" max="38" width="11.7109375" customWidth="1"/>
+    <col min="39" max="39" width="15.5703125" customWidth="1"/>
+    <col min="40" max="40" width="16.28515625" customWidth="1"/>
+    <col min="41" max="41" width="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:41" x14ac:dyDescent="0.25">
@@ -14273,113 +14297,208 @@
       <c r="B12" s="93" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="110"/>
-      <c r="D12" s="110"/>
-      <c r="E12" s="110"/>
-      <c r="F12" s="110"/>
-      <c r="G12" s="93"/>
-      <c r="H12" s="93"/>
-      <c r="I12" s="93"/>
-      <c r="J12" s="93"/>
-      <c r="K12" s="93"/>
-      <c r="L12" s="93"/>
-      <c r="M12" s="93"/>
-      <c r="N12" s="93"/>
-      <c r="O12" s="93"/>
-      <c r="P12" s="93"/>
-      <c r="Q12" s="93"/>
-      <c r="R12" s="93"/>
-      <c r="S12" s="18"/>
-      <c r="T12" s="18"/>
-      <c r="U12" s="18"/>
-      <c r="Z12" s="32" t="e">
+      <c r="C12" s="110">
+        <v>11209.395989000001</v>
+      </c>
+      <c r="D12" s="110">
+        <v>124.898977</v>
+      </c>
+      <c r="E12" s="110">
+        <v>4937.9413530000002</v>
+      </c>
+      <c r="F12" s="110">
+        <v>1.2490000000000001</v>
+      </c>
+      <c r="G12" s="93">
+        <v>1.2490000000000001</v>
+      </c>
+      <c r="H12" s="93">
+        <v>0.60299999999999998</v>
+      </c>
+      <c r="I12" s="93">
+        <v>0.60299999999999998</v>
+      </c>
+      <c r="J12" s="93">
+        <v>0</v>
+      </c>
+      <c r="K12" s="93">
+        <v>0.98399999999999999</v>
+      </c>
+      <c r="L12" s="93">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="M12" s="93">
+        <v>0.01</v>
+      </c>
+      <c r="N12" s="93">
+        <v>0.19600000000000001</v>
+      </c>
+      <c r="O12" s="93">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="P12" s="93">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="Q12" s="93">
+        <v>1E-3</v>
+      </c>
+      <c r="R12" s="93">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="S12" s="18">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="T12" s="18">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="U12" s="18">
+        <v>0.54</v>
+      </c>
+      <c r="Z12" s="32">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AA12" s="32" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AB12" s="32" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC12" s="32" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AD12" s="32" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AE12" s="32" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AF12" s="32" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AG12" s="32" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AH12" s="32" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AI12" s="32" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AJ12" s="32" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK12" s="32" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AL12" s="32" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AM12" s="32" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AN12" s="32" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AO12" s="32" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>1167.2296666666664</v>
+      </c>
+      <c r="AA12" s="32">
+        <f t="shared" si="0"/>
+        <v>127.098</v>
+      </c>
+      <c r="AB12" s="32">
+        <f t="shared" si="0"/>
+        <v>40.029666666666664</v>
+      </c>
+      <c r="AC12" s="32">
+        <f t="shared" si="0"/>
+        <v>35.514333333333333</v>
+      </c>
+      <c r="AD12" s="32">
+        <f t="shared" si="0"/>
+        <v>11.523333333333333</v>
+      </c>
+      <c r="AE12" s="32">
+        <f t="shared" si="0"/>
+        <v>0.62133333333333329</v>
+      </c>
+      <c r="AF12" s="32">
+        <f t="shared" si="0"/>
+        <v>9.6666666666666679E-2</v>
+      </c>
+      <c r="AG12" s="32">
+        <f t="shared" si="0"/>
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="AH12" s="32">
+        <f t="shared" si="0"/>
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="AI12" s="32">
+        <f t="shared" si="0"/>
+        <v>2.5666666666666667E-2</v>
+      </c>
+      <c r="AJ12" s="32">
+        <f t="shared" si="0"/>
+        <v>5.3333333333333332E-3</v>
+      </c>
+      <c r="AK12" s="32">
+        <f t="shared" si="0"/>
+        <v>3.3333333333333332E-4</v>
+      </c>
+      <c r="AL12" s="32">
+        <f t="shared" si="0"/>
+        <v>0.10666666666666667</v>
+      </c>
+      <c r="AM12" s="32">
+        <f t="shared" si="0"/>
+        <v>0.18266666666666667</v>
+      </c>
+      <c r="AN12" s="32">
+        <f t="shared" si="0"/>
+        <v>0.10966666666666668</v>
+      </c>
+      <c r="AO12" s="32">
+        <f t="shared" si="0"/>
+        <v>0.35866666666666669</v>
       </c>
     </row>
     <row r="13" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B13" s="114" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
-      <c r="P13" s="4"/>
-      <c r="Q13" s="4"/>
-      <c r="R13" s="4"/>
-      <c r="S13" s="4"/>
-      <c r="T13" s="4"/>
-      <c r="U13" s="4"/>
+      <c r="C13" s="4">
+        <f>AVERAGE(C4:C12)</f>
+        <v>4461931.0639908891</v>
+      </c>
+      <c r="D13" s="4">
+        <f t="shared" ref="D13:U13" si="2">AVERAGE(D4:D12)</f>
+        <v>11630.232610444444</v>
+      </c>
+      <c r="E13" s="4">
+        <f t="shared" si="2"/>
+        <v>233018.41779411113</v>
+      </c>
+      <c r="F13" s="4">
+        <f t="shared" si="2"/>
+        <v>13.649444444444445</v>
+      </c>
+      <c r="G13" s="4">
+        <f t="shared" si="2"/>
+        <v>12.311777777777777</v>
+      </c>
+      <c r="H13" s="4">
+        <f t="shared" si="2"/>
+        <v>5.2326666666666668</v>
+      </c>
+      <c r="I13" s="4">
+        <f t="shared" si="2"/>
+        <v>5.1897777777777785</v>
+      </c>
+      <c r="J13" s="4">
+        <f t="shared" si="2"/>
+        <v>5.6666666666666671E-2</v>
+      </c>
+      <c r="K13" s="4">
+        <f t="shared" si="2"/>
+        <v>0.92233333333333334</v>
+      </c>
+      <c r="L13" s="4">
+        <f t="shared" si="2"/>
+        <v>2.2555555555555561E-2</v>
+      </c>
+      <c r="M13" s="4">
+        <f t="shared" si="2"/>
+        <v>8.8444444444444451E-2</v>
+      </c>
+      <c r="N13" s="4">
+        <f t="shared" si="2"/>
+        <v>7.2000000000000008E-2</v>
+      </c>
+      <c r="O13" s="4">
+        <f t="shared" si="2"/>
+        <v>0.14066666666666663</v>
+      </c>
+      <c r="P13" s="4">
+        <f t="shared" si="2"/>
+        <v>1.6666666666666666E-3</v>
+      </c>
+      <c r="Q13" s="4">
+        <f t="shared" si="2"/>
+        <v>1.1111111111111112E-4</v>
+      </c>
+      <c r="R13" s="4">
+        <f t="shared" si="2"/>
+        <v>9.8888888888888898E-3</v>
+      </c>
+      <c r="S13" s="4">
+        <f t="shared" si="2"/>
+        <v>0.16844444444444445</v>
+      </c>
+      <c r="T13" s="4">
+        <f t="shared" si="2"/>
+        <v>3.7666666666666668E-2</v>
+      </c>
+      <c r="U13" s="4">
+        <f t="shared" si="2"/>
+        <v>0.45844444444444438</v>
+      </c>
     </row>
     <row r="14" spans="2:41" x14ac:dyDescent="0.25">
       <c r="C14" s="2"/>
@@ -15031,25 +15150,63 @@
       <c r="B28" s="93" t="s">
         <v>8</v>
       </c>
-      <c r="C28" s="110"/>
-      <c r="D28" s="110"/>
-      <c r="E28" s="110"/>
-      <c r="F28" s="110"/>
-      <c r="G28" s="93"/>
-      <c r="H28" s="93"/>
-      <c r="I28" s="93"/>
-      <c r="J28" s="93"/>
-      <c r="K28" s="93"/>
-      <c r="L28" s="93"/>
-      <c r="M28" s="93"/>
-      <c r="N28" s="93"/>
-      <c r="O28" s="93"/>
-      <c r="P28" s="93"/>
-      <c r="Q28" s="93"/>
-      <c r="R28" s="93"/>
-      <c r="S28" s="18"/>
-      <c r="T28" s="18"/>
-      <c r="U28" s="18"/>
+      <c r="C28" s="110">
+        <v>15771.716541</v>
+      </c>
+      <c r="D28" s="110">
+        <v>11590.733367000001</v>
+      </c>
+      <c r="E28" s="110">
+        <v>60695.630100000002</v>
+      </c>
+      <c r="F28" s="110">
+        <v>2790.3359999999998</v>
+      </c>
+      <c r="G28" s="93">
+        <v>190.35</v>
+      </c>
+      <c r="H28" s="93">
+        <v>55.155999999999999</v>
+      </c>
+      <c r="I28" s="93">
+        <v>46.994999999999997</v>
+      </c>
+      <c r="J28" s="93">
+        <v>17.97</v>
+      </c>
+      <c r="K28" s="93">
+        <v>0.63700000000000001</v>
+      </c>
+      <c r="L28" s="93">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="M28" s="93">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="N28" s="93">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="O28" s="93">
+        <v>0</v>
+      </c>
+      <c r="P28" s="93">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="93">
+        <v>0</v>
+      </c>
+      <c r="R28" s="93">
+        <v>0.157</v>
+      </c>
+      <c r="S28" s="18">
+        <v>0.253</v>
+      </c>
+      <c r="T28" s="18">
+        <v>0.123</v>
+      </c>
+      <c r="U28" s="18">
+        <v>0.224</v>
+      </c>
       <c r="W28" t="s">
         <v>37</v>
       </c>
@@ -15058,25 +15215,82 @@
       <c r="B29" s="114" t="s">
         <v>33</v>
       </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
-      <c r="L29" s="4"/>
-      <c r="M29" s="4"/>
-      <c r="N29" s="4"/>
-      <c r="O29" s="4"/>
-      <c r="P29" s="4"/>
-      <c r="Q29" s="4"/>
-      <c r="R29" s="4"/>
-      <c r="S29" s="4"/>
-      <c r="T29" s="4"/>
-      <c r="U29" s="4"/>
+      <c r="C29" s="4">
+        <f>AVERAGE(C20:C28)</f>
+        <v>54244.68228666667</v>
+      </c>
+      <c r="D29" s="4">
+        <f t="shared" ref="D29:U29" si="3">AVERAGE(D20:D28)</f>
+        <v>8464.0604963333335</v>
+      </c>
+      <c r="E29" s="4">
+        <f t="shared" si="3"/>
+        <v>31826.202315666673</v>
+      </c>
+      <c r="F29" s="4">
+        <f t="shared" si="3"/>
+        <v>997.69688888888902</v>
+      </c>
+      <c r="G29" s="4">
+        <f t="shared" si="3"/>
+        <v>39.555888888888887</v>
+      </c>
+      <c r="H29" s="4">
+        <f t="shared" si="3"/>
+        <v>13.723333333333333</v>
+      </c>
+      <c r="I29" s="4">
+        <f t="shared" si="3"/>
+        <v>12.418222222222223</v>
+      </c>
+      <c r="J29" s="4">
+        <f t="shared" si="3"/>
+        <v>2.4988888888888887</v>
+      </c>
+      <c r="K29" s="4">
+        <f t="shared" si="3"/>
+        <v>0.76611111111111108</v>
+      </c>
+      <c r="L29" s="4">
+        <f t="shared" si="3"/>
+        <v>5.3666666666666668E-2</v>
+      </c>
+      <c r="M29" s="4">
+        <f t="shared" si="3"/>
+        <v>0.18033333333333335</v>
+      </c>
+      <c r="N29" s="4">
+        <f t="shared" si="3"/>
+        <v>1.2986666666666666</v>
+      </c>
+      <c r="O29" s="4">
+        <f t="shared" si="3"/>
+        <v>0.16233333333333333</v>
+      </c>
+      <c r="P29" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Q29" s="4">
+        <f t="shared" si="3"/>
+        <v>4.4444444444444447E-4</v>
+      </c>
+      <c r="R29" s="4">
+        <f t="shared" si="3"/>
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="S29" s="4">
+        <f t="shared" si="3"/>
+        <v>0.10077777777777777</v>
+      </c>
+      <c r="T29" s="4">
+        <f t="shared" si="3"/>
+        <v>9.0444444444444452E-2</v>
+      </c>
+      <c r="U29" s="4">
+        <f t="shared" si="3"/>
+        <v>8.0111111111111105E-2</v>
+      </c>
       <c r="W29" t="s">
         <v>31</v>
       </c>
@@ -15715,49 +15929,144 @@
       <c r="B44" s="93" t="s">
         <v>8</v>
       </c>
-      <c r="C44" s="110"/>
-      <c r="D44" s="110"/>
-      <c r="E44" s="110"/>
-      <c r="F44" s="110"/>
-      <c r="G44" s="93"/>
-      <c r="H44" s="93"/>
-      <c r="I44" s="93"/>
-      <c r="J44" s="93"/>
-      <c r="K44" s="93"/>
-      <c r="L44" s="93"/>
-      <c r="M44" s="93"/>
-      <c r="N44" s="93"/>
-      <c r="O44" s="93"/>
-      <c r="P44" s="93"/>
-      <c r="Q44" s="93"/>
-      <c r="R44" s="93"/>
-      <c r="S44" s="18"/>
-      <c r="T44" s="18"/>
-      <c r="U44" s="18"/>
+      <c r="C44" s="110">
+        <v>1991.068724</v>
+      </c>
+      <c r="D44" s="110">
+        <v>1867.7162370000001</v>
+      </c>
+      <c r="E44" s="110">
+        <v>3943.0801900000001</v>
+      </c>
+      <c r="F44" s="110">
+        <v>710.10400000000004</v>
+      </c>
+      <c r="G44" s="93">
+        <v>189.69499999999999</v>
+      </c>
+      <c r="H44" s="93">
+        <v>64.33</v>
+      </c>
+      <c r="I44" s="93">
+        <v>58.945</v>
+      </c>
+      <c r="J44" s="93">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="K44" s="93">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="L44" s="93">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="M44" s="93">
+        <v>2E-3</v>
+      </c>
+      <c r="N44" s="93">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="O44" s="93">
+        <v>0</v>
+      </c>
+      <c r="P44" s="93">
+        <v>1E-3</v>
+      </c>
+      <c r="Q44" s="93">
+        <v>0</v>
+      </c>
+      <c r="R44" s="93">
+        <v>0.16</v>
+      </c>
+      <c r="S44" s="18">
+        <v>0.21099999999999999</v>
+      </c>
+      <c r="T44" s="18">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="U44" s="18">
+        <v>0.312</v>
+      </c>
     </row>
     <row r="45" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B45" s="114" t="s">
         <v>33</v>
       </c>
-      <c r="C45" s="4"/>
-      <c r="D45" s="4"/>
-      <c r="E45" s="4"/>
-      <c r="F45" s="4"/>
-      <c r="G45" s="4"/>
-      <c r="H45" s="4"/>
-      <c r="I45" s="4"/>
-      <c r="J45" s="4"/>
-      <c r="K45" s="4"/>
-      <c r="L45" s="4"/>
-      <c r="M45" s="4"/>
-      <c r="N45" s="4"/>
-      <c r="O45" s="4"/>
-      <c r="P45" s="4"/>
-      <c r="Q45" s="4"/>
-      <c r="R45" s="4"/>
-      <c r="S45" s="4"/>
-      <c r="T45" s="4"/>
-      <c r="U45" s="4"/>
+      <c r="C45" s="4">
+        <f>AVERAGE(C36:C44)</f>
+        <v>29323.690055888888</v>
+      </c>
+      <c r="D45" s="4">
+        <f t="shared" ref="D45:U45" si="4">AVERAGE(D36:D44)</f>
+        <v>1816.9407325555558</v>
+      </c>
+      <c r="E45" s="4">
+        <f t="shared" si="4"/>
+        <v>4552.6785966666675</v>
+      </c>
+      <c r="F45" s="4">
+        <f t="shared" si="4"/>
+        <v>122.54077777777781</v>
+      </c>
+      <c r="G45" s="4">
+        <f t="shared" si="4"/>
+        <v>45.721111111111114</v>
+      </c>
+      <c r="H45" s="4">
+        <f t="shared" si="4"/>
+        <v>17.080777777777779</v>
+      </c>
+      <c r="I45" s="4">
+        <f t="shared" si="4"/>
+        <v>16.071666666666669</v>
+      </c>
+      <c r="J45" s="4">
+        <f t="shared" si="4"/>
+        <v>2.4255555555555559</v>
+      </c>
+      <c r="K45" s="4">
+        <f t="shared" si="4"/>
+        <v>0.66711111111111121</v>
+      </c>
+      <c r="L45" s="4">
+        <f t="shared" si="4"/>
+        <v>5.4666666666666669E-2</v>
+      </c>
+      <c r="M45" s="4">
+        <f t="shared" si="4"/>
+        <v>0.16322222222222224</v>
+      </c>
+      <c r="N45" s="4">
+        <f t="shared" si="4"/>
+        <v>2.0111111111111111E-2</v>
+      </c>
+      <c r="O45" s="4">
+        <f t="shared" si="4"/>
+        <v>0.25211111111111106</v>
+      </c>
+      <c r="P45" s="4">
+        <f t="shared" si="4"/>
+        <v>1.1111111111111112E-4</v>
+      </c>
+      <c r="Q45" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R45" s="4">
+        <f t="shared" si="4"/>
+        <v>4.1222222222222223E-2</v>
+      </c>
+      <c r="S45" s="4">
+        <f t="shared" si="4"/>
+        <v>9.0777777777777791E-2</v>
+      </c>
+      <c r="T45" s="4">
+        <f t="shared" si="4"/>
+        <v>0.27066666666666667</v>
+      </c>
+      <c r="U45" s="4">
+        <f t="shared" si="4"/>
+        <v>0.10677777777777779</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="42">
@@ -15806,4 +16115,2547 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:AO46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="V44" sqref="V44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="4.42578125" customWidth="1"/>
+    <col min="4" max="4" width="3" customWidth="1"/>
+    <col min="5" max="5" width="3.28515625" customWidth="1"/>
+    <col min="6" max="6" width="3" customWidth="1"/>
+    <col min="7" max="7" width="3.42578125" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" customWidth="1"/>
+    <col min="9" max="9" width="5" customWidth="1"/>
+    <col min="10" max="10" width="4.42578125" customWidth="1"/>
+    <col min="11" max="11" width="2" customWidth="1"/>
+    <col min="12" max="12" width="9.85546875" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" customWidth="1"/>
+    <col min="14" max="14" width="10.85546875" customWidth="1"/>
+    <col min="15" max="15" width="11.140625" customWidth="1"/>
+    <col min="16" max="16" width="14.5703125" customWidth="1"/>
+    <col min="17" max="18" width="10.85546875" customWidth="1"/>
+    <col min="19" max="20" width="16.42578125" customWidth="1"/>
+    <col min="21" max="21" width="17.5703125" customWidth="1"/>
+    <col min="26" max="26" width="10.5703125" customWidth="1"/>
+    <col min="27" max="27" width="12.42578125" customWidth="1"/>
+    <col min="28" max="28" width="11.140625" customWidth="1"/>
+    <col min="29" max="29" width="21.28515625" customWidth="1"/>
+    <col min="30" max="30" width="13.7109375" customWidth="1"/>
+    <col min="31" max="31" width="10.5703125" customWidth="1"/>
+    <col min="32" max="32" width="11" customWidth="1"/>
+    <col min="33" max="33" width="10.5703125" customWidth="1"/>
+    <col min="36" max="36" width="11.85546875" customWidth="1"/>
+    <col min="38" max="38" width="11.7109375" customWidth="1"/>
+    <col min="39" max="39" width="15.5703125" customWidth="1"/>
+    <col min="40" max="40" width="16.28515625" customWidth="1"/>
+    <col min="41" max="41" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:41" x14ac:dyDescent="0.25">
+      <c r="B1" s="137" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="138"/>
+      <c r="D1" s="138"/>
+      <c r="E1" s="138"/>
+      <c r="F1" s="138"/>
+      <c r="G1" s="138"/>
+      <c r="H1" s="138"/>
+      <c r="I1" s="138"/>
+      <c r="J1" s="138"/>
+      <c r="K1" s="138"/>
+      <c r="L1" s="138"/>
+      <c r="M1" s="138"/>
+      <c r="N1" s="138"/>
+      <c r="O1" s="138"/>
+      <c r="P1" s="138"/>
+      <c r="Q1" s="138"/>
+      <c r="R1" s="139"/>
+      <c r="Z1" s="126" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA1" s="127"/>
+      <c r="AB1" s="127"/>
+      <c r="AC1" s="127"/>
+      <c r="AD1" s="127"/>
+      <c r="AE1" s="128"/>
+    </row>
+    <row r="2" spans="2:41" x14ac:dyDescent="0.25">
+      <c r="B2" s="99" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="126" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="127" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="127" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="127" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="127" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="127" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="127" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="127" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" s="128" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="129" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" s="122"/>
+      <c r="N2" s="122"/>
+      <c r="O2" s="122"/>
+      <c r="P2" s="122"/>
+      <c r="Q2" s="122"/>
+      <c r="R2" s="122"/>
+      <c r="S2" s="127"/>
+      <c r="T2" s="127"/>
+      <c r="U2" s="128"/>
+      <c r="Z2" s="129" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA2" s="122" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB2" s="122" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC2" s="122" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD2" s="122" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE2" s="123" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF2" s="129" t="s">
+        <v>25</v>
+      </c>
+      <c r="AG2" s="122"/>
+      <c r="AH2" s="122"/>
+      <c r="AI2" s="122"/>
+      <c r="AJ2" s="122"/>
+      <c r="AK2" s="122"/>
+      <c r="AL2" s="122"/>
+      <c r="AM2" s="127"/>
+      <c r="AN2" s="127"/>
+      <c r="AO2" s="128"/>
+    </row>
+    <row r="3" spans="2:41" x14ac:dyDescent="0.25">
+      <c r="B3" s="100"/>
+      <c r="C3" s="130"/>
+      <c r="D3" s="124"/>
+      <c r="E3" s="124"/>
+      <c r="F3" s="124"/>
+      <c r="G3" s="124"/>
+      <c r="H3" s="124"/>
+      <c r="I3" s="124"/>
+      <c r="J3" s="124"/>
+      <c r="K3" s="125"/>
+      <c r="L3" s="111" t="s">
+        <v>18</v>
+      </c>
+      <c r="M3" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="N3" s="56" t="s">
+        <v>20</v>
+      </c>
+      <c r="O3" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="P3" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q3" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="R3" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="S3" s="112" t="s">
+        <v>39</v>
+      </c>
+      <c r="T3" s="112" t="s">
+        <v>40</v>
+      </c>
+      <c r="U3" s="113" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z3" s="130"/>
+      <c r="AA3" s="124"/>
+      <c r="AB3" s="124"/>
+      <c r="AC3" s="124"/>
+      <c r="AD3" s="124"/>
+      <c r="AE3" s="125"/>
+      <c r="AF3" s="111" t="s">
+        <v>18</v>
+      </c>
+      <c r="AG3" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="AH3" s="56" t="s">
+        <v>20</v>
+      </c>
+      <c r="AI3" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ3" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="AK3" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="AL3" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="AM3" s="112" t="s">
+        <v>39</v>
+      </c>
+      <c r="AN3" s="112" t="s">
+        <v>40</v>
+      </c>
+      <c r="AO3" s="113" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="2:41" x14ac:dyDescent="0.25">
+      <c r="B4" s="101" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="102"/>
+      <c r="D4" s="102"/>
+      <c r="E4" s="102"/>
+      <c r="F4" s="101"/>
+      <c r="G4" s="101"/>
+      <c r="H4" s="101">
+        <v>8.9060000000000006</v>
+      </c>
+      <c r="I4" s="101"/>
+      <c r="J4" s="101"/>
+      <c r="K4" s="101"/>
+      <c r="L4" s="101">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="M4" s="101">
+        <v>2E-3</v>
+      </c>
+      <c r="N4" s="101">
+        <v>3.1E-2</v>
+      </c>
+      <c r="O4" s="101">
+        <v>0.51600000000000001</v>
+      </c>
+      <c r="P4" s="101">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="101">
+        <v>0</v>
+      </c>
+      <c r="R4" s="101">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="S4" s="6">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="T4" s="6">
+        <v>0.108</v>
+      </c>
+      <c r="U4" s="6">
+        <v>0.105</v>
+      </c>
+      <c r="Z4" s="24"/>
+      <c r="AA4" s="24"/>
+      <c r="AB4" s="24">
+        <f t="shared" ref="AA4:AO12" si="0">AVERAGE(H4,H20,H36)</f>
+        <v>16.416666666666668</v>
+      </c>
+      <c r="AC4" s="24"/>
+      <c r="AD4" s="24"/>
+      <c r="AE4" s="24"/>
+      <c r="AF4" s="24">
+        <f t="shared" si="0"/>
+        <v>7.8E-2</v>
+      </c>
+      <c r="AG4" s="24">
+        <f t="shared" si="0"/>
+        <v>1E-3</v>
+      </c>
+      <c r="AH4" s="24">
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001E-2</v>
+      </c>
+      <c r="AI4" s="24">
+        <f t="shared" si="0"/>
+        <v>0.22366666666666668</v>
+      </c>
+      <c r="AJ4" s="24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AK4" s="24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AL4" s="24">
+        <f t="shared" si="0"/>
+        <v>4.5666666666666661E-2</v>
+      </c>
+      <c r="AM4" s="24">
+        <f t="shared" si="0"/>
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="AN4" s="24">
+        <f t="shared" si="0"/>
+        <v>0.44266666666666671</v>
+      </c>
+      <c r="AO4" s="24">
+        <f t="shared" si="0"/>
+        <v>9.3333333333333338E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:41" x14ac:dyDescent="0.25">
+      <c r="B5" s="72" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="103"/>
+      <c r="D5" s="103"/>
+      <c r="E5" s="103"/>
+      <c r="F5" s="103"/>
+      <c r="G5" s="72"/>
+      <c r="H5" s="72">
+        <v>6.2510000000000003</v>
+      </c>
+      <c r="I5" s="72"/>
+      <c r="J5" s="72"/>
+      <c r="K5" s="72"/>
+      <c r="L5" s="72">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="M5" s="72">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="N5" s="72">
+        <v>0.182</v>
+      </c>
+      <c r="O5" s="72">
+        <v>0.17899999999999999</v>
+      </c>
+      <c r="P5" s="72">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="72">
+        <v>0</v>
+      </c>
+      <c r="R5" s="72">
+        <v>1E-3</v>
+      </c>
+      <c r="S5" s="8">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="T5" s="8">
+        <v>0.127</v>
+      </c>
+      <c r="U5" s="8">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="Z5" s="25"/>
+      <c r="AA5" s="25"/>
+      <c r="AB5" s="25">
+        <f t="shared" si="0"/>
+        <v>10.35</v>
+      </c>
+      <c r="AC5" s="25"/>
+      <c r="AD5" s="25"/>
+      <c r="AE5" s="25"/>
+      <c r="AF5" s="25">
+        <f t="shared" si="0"/>
+        <v>1.8333333333333333E-2</v>
+      </c>
+      <c r="AG5" s="25">
+        <f t="shared" si="0"/>
+        <v>0.27733333333333338</v>
+      </c>
+      <c r="AH5" s="25">
+        <f t="shared" si="0"/>
+        <v>0.36633333333333334</v>
+      </c>
+      <c r="AI5" s="25">
+        <f t="shared" si="0"/>
+        <v>0.19199999999999998</v>
+      </c>
+      <c r="AJ5" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AK5" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AL5" s="25">
+        <f t="shared" si="0"/>
+        <v>4.333333333333334E-3</v>
+      </c>
+      <c r="AM5" s="25">
+        <f t="shared" si="0"/>
+        <v>7.7666666666666662E-2</v>
+      </c>
+      <c r="AN5" s="25">
+        <f t="shared" si="0"/>
+        <v>7.4333333333333335E-2</v>
+      </c>
+      <c r="AO5" s="25">
+        <f t="shared" si="0"/>
+        <v>6.8666666666666668E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:41" x14ac:dyDescent="0.25">
+      <c r="B6" s="75" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="104"/>
+      <c r="D6" s="104"/>
+      <c r="E6" s="104"/>
+      <c r="F6" s="104"/>
+      <c r="G6" s="75"/>
+      <c r="H6" s="75">
+        <v>16.245999999999999</v>
+      </c>
+      <c r="I6" s="75"/>
+      <c r="J6" s="75"/>
+      <c r="K6" s="75"/>
+      <c r="L6" s="75">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="M6" s="75">
+        <v>1E-3</v>
+      </c>
+      <c r="N6" s="75">
+        <v>0</v>
+      </c>
+      <c r="O6" s="75">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="P6" s="75">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="75">
+        <v>0</v>
+      </c>
+      <c r="R6" s="75">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="S6" s="10">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="T6" s="10">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="U6" s="10">
+        <v>0.63800000000000001</v>
+      </c>
+      <c r="Z6" s="26"/>
+      <c r="AA6" s="26"/>
+      <c r="AB6" s="26">
+        <f t="shared" si="0"/>
+        <v>10.909999999999998</v>
+      </c>
+      <c r="AC6" s="26"/>
+      <c r="AD6" s="26"/>
+      <c r="AE6" s="26"/>
+      <c r="AF6" s="26">
+        <f t="shared" si="0"/>
+        <v>0.10166666666666667</v>
+      </c>
+      <c r="AG6" s="26">
+        <f t="shared" si="0"/>
+        <v>2.6666666666666666E-3</v>
+      </c>
+      <c r="AH6" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AI6" s="26">
+        <f t="shared" si="0"/>
+        <v>0.34666666666666668</v>
+      </c>
+      <c r="AJ6" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AK6" s="26">
+        <f t="shared" si="0"/>
+        <v>6.6666666666666664E-4</v>
+      </c>
+      <c r="AL6" s="26">
+        <f t="shared" si="0"/>
+        <v>5.9666666666666666E-2</v>
+      </c>
+      <c r="AM6" s="26">
+        <f t="shared" si="0"/>
+        <v>0.12833333333333333</v>
+      </c>
+      <c r="AN6" s="26">
+        <f t="shared" si="0"/>
+        <v>5.8333333333333341E-2</v>
+      </c>
+      <c r="AO6" s="26">
+        <f t="shared" si="0"/>
+        <v>0.30166666666666669</v>
+      </c>
+    </row>
+    <row r="7" spans="2:41" x14ac:dyDescent="0.25">
+      <c r="B7" s="78" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="105"/>
+      <c r="D7" s="105"/>
+      <c r="E7" s="105"/>
+      <c r="F7" s="105"/>
+      <c r="G7" s="78"/>
+      <c r="H7" s="78">
+        <v>9.7149999999999999</v>
+      </c>
+      <c r="I7" s="78"/>
+      <c r="J7" s="78"/>
+      <c r="K7" s="78"/>
+      <c r="L7" s="78">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="M7" s="78">
+        <v>0.39800000000000002</v>
+      </c>
+      <c r="N7" s="78">
+        <v>0.2</v>
+      </c>
+      <c r="O7" s="78">
+        <v>0.39700000000000002</v>
+      </c>
+      <c r="P7" s="78">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="78">
+        <v>0</v>
+      </c>
+      <c r="R7" s="78">
+        <v>1E-3</v>
+      </c>
+      <c r="S7" s="12">
+        <v>0</v>
+      </c>
+      <c r="T7" s="12">
+        <v>0</v>
+      </c>
+      <c r="U7" s="12">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="27"/>
+      <c r="AA7" s="27"/>
+      <c r="AB7" s="27">
+        <f t="shared" si="0"/>
+        <v>13.863999999999999</v>
+      </c>
+      <c r="AC7" s="27"/>
+      <c r="AD7" s="27"/>
+      <c r="AE7" s="27"/>
+      <c r="AF7" s="27">
+        <f t="shared" si="0"/>
+        <v>6.0333333333333329E-2</v>
+      </c>
+      <c r="AG7" s="27">
+        <f t="shared" si="0"/>
+        <v>0.48299999999999993</v>
+      </c>
+      <c r="AH7" s="27">
+        <f t="shared" si="0"/>
+        <v>0.12766666666666668</v>
+      </c>
+      <c r="AI7" s="27">
+        <f t="shared" si="0"/>
+        <v>0.25266666666666671</v>
+      </c>
+      <c r="AJ7" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AK7" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AL7" s="27">
+        <f t="shared" si="0"/>
+        <v>7.6666666666666675E-2</v>
+      </c>
+      <c r="AM7" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AN7" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AO7" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:41" x14ac:dyDescent="0.25">
+      <c r="B8" s="81" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="106"/>
+      <c r="D8" s="106"/>
+      <c r="E8" s="106"/>
+      <c r="F8" s="106"/>
+      <c r="G8" s="81"/>
+      <c r="H8" s="81">
+        <v>0.33200000000000002</v>
+      </c>
+      <c r="I8" s="81"/>
+      <c r="J8" s="81"/>
+      <c r="K8" s="81"/>
+      <c r="L8" s="81">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="M8" s="81">
+        <v>1E-3</v>
+      </c>
+      <c r="N8" s="81">
+        <v>0.51100000000000001</v>
+      </c>
+      <c r="O8" s="81">
+        <v>7.8E-2</v>
+      </c>
+      <c r="P8" s="81">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="81">
+        <v>0</v>
+      </c>
+      <c r="R8" s="81">
+        <v>1E-3</v>
+      </c>
+      <c r="S8" s="20">
+        <v>0.32900000000000001</v>
+      </c>
+      <c r="T8" s="20">
+        <v>0.03</v>
+      </c>
+      <c r="U8" s="20">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="Z8" s="28"/>
+      <c r="AA8" s="28"/>
+      <c r="AB8" s="28">
+        <f t="shared" si="0"/>
+        <v>1.8103333333333333</v>
+      </c>
+      <c r="AC8" s="28"/>
+      <c r="AD8" s="28"/>
+      <c r="AE8" s="28"/>
+      <c r="AF8" s="28">
+        <f t="shared" si="0"/>
+        <v>9.3333333333333341E-3</v>
+      </c>
+      <c r="AG8" s="28">
+        <f t="shared" si="0"/>
+        <v>0.33833333333333332</v>
+      </c>
+      <c r="AH8" s="28">
+        <f t="shared" si="0"/>
+        <v>0.18800000000000003</v>
+      </c>
+      <c r="AI8" s="28">
+        <f t="shared" si="0"/>
+        <v>0.29099999999999998</v>
+      </c>
+      <c r="AJ8" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AK8" s="28">
+        <f t="shared" si="0"/>
+        <v>3.3333333333333332E-4</v>
+      </c>
+      <c r="AL8" s="28">
+        <f t="shared" si="0"/>
+        <v>6.6666666666666664E-4</v>
+      </c>
+      <c r="AM8" s="28">
+        <f t="shared" si="0"/>
+        <v>0.12266666666666666</v>
+      </c>
+      <c r="AN8" s="28">
+        <f t="shared" si="0"/>
+        <v>2.2000000000000002E-2</v>
+      </c>
+      <c r="AO8" s="28">
+        <f t="shared" si="0"/>
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:41" x14ac:dyDescent="0.25">
+      <c r="B9" s="84" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="107"/>
+      <c r="D9" s="107"/>
+      <c r="E9" s="107"/>
+      <c r="F9" s="107"/>
+      <c r="G9" s="84"/>
+      <c r="H9" s="84">
+        <v>5.34</v>
+      </c>
+      <c r="I9" s="84"/>
+      <c r="J9" s="84"/>
+      <c r="K9" s="84"/>
+      <c r="L9" s="84">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="M9" s="84">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="N9" s="84">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="O9" s="84">
+        <v>0.53200000000000003</v>
+      </c>
+      <c r="P9" s="84">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="84">
+        <v>0</v>
+      </c>
+      <c r="R9" s="84">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="S9" s="16">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="T9" s="16">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="U9" s="16">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="Z9" s="29"/>
+      <c r="AA9" s="29"/>
+      <c r="AB9" s="29">
+        <f t="shared" si="0"/>
+        <v>5.2440000000000007</v>
+      </c>
+      <c r="AC9" s="29"/>
+      <c r="AD9" s="29"/>
+      <c r="AE9" s="29"/>
+      <c r="AF9" s="29">
+        <f t="shared" si="0"/>
+        <v>2.0666666666666667E-2</v>
+      </c>
+      <c r="AG9" s="29">
+        <f t="shared" si="0"/>
+        <v>0.36400000000000005</v>
+      </c>
+      <c r="AH9" s="29">
+        <f t="shared" si="0"/>
+        <v>9.0000000000000011E-3</v>
+      </c>
+      <c r="AI9" s="29">
+        <f t="shared" si="0"/>
+        <v>0.38800000000000007</v>
+      </c>
+      <c r="AJ9" s="29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AK9" s="29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AL9" s="29">
+        <f t="shared" si="0"/>
+        <v>3.6666666666666666E-3</v>
+      </c>
+      <c r="AM9" s="29">
+        <f t="shared" si="0"/>
+        <v>9.7333333333333327E-2</v>
+      </c>
+      <c r="AN9" s="29">
+        <f t="shared" si="0"/>
+        <v>6.2666666666666662E-2</v>
+      </c>
+      <c r="AO9" s="29">
+        <f t="shared" si="0"/>
+        <v>5.1666666666666666E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:41" x14ac:dyDescent="0.25">
+      <c r="B10" s="87" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="108"/>
+      <c r="D10" s="108"/>
+      <c r="E10" s="108"/>
+      <c r="F10" s="108"/>
+      <c r="G10" s="87"/>
+      <c r="H10" s="87">
+        <v>0.73099999999999998</v>
+      </c>
+      <c r="I10" s="87"/>
+      <c r="J10" s="87"/>
+      <c r="K10" s="87"/>
+      <c r="L10" s="87">
+        <v>0.83199999999999996</v>
+      </c>
+      <c r="M10" s="87">
+        <v>0</v>
+      </c>
+      <c r="N10" s="87">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="O10" s="87">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="P10" s="87">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="87">
+        <v>0</v>
+      </c>
+      <c r="R10" s="87">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="S10" s="14">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="T10" s="14">
+        <v>1.2E-2</v>
+      </c>
+      <c r="U10" s="14">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="Z10" s="30"/>
+      <c r="AA10" s="30"/>
+      <c r="AB10" s="30">
+        <f t="shared" si="0"/>
+        <v>4.88</v>
+      </c>
+      <c r="AC10" s="30"/>
+      <c r="AD10" s="30"/>
+      <c r="AE10" s="30"/>
+      <c r="AF10" s="30">
+        <f t="shared" si="0"/>
+        <v>0.32866666666666666</v>
+      </c>
+      <c r="AG10" s="30">
+        <f t="shared" si="0"/>
+        <v>9.1666666666666674E-2</v>
+      </c>
+      <c r="AH10" s="30">
+        <f t="shared" si="0"/>
+        <v>0.13966666666666666</v>
+      </c>
+      <c r="AI10" s="30">
+        <f t="shared" si="0"/>
+        <v>0.32866666666666666</v>
+      </c>
+      <c r="AJ10" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AK10" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AL10" s="30">
+        <f t="shared" si="0"/>
+        <v>5.6666666666666671E-3</v>
+      </c>
+      <c r="AM10" s="30">
+        <f t="shared" si="0"/>
+        <v>5.3333333333333337E-2</v>
+      </c>
+      <c r="AN10" s="30">
+        <f t="shared" si="0"/>
+        <v>2.9666666666666664E-2</v>
+      </c>
+      <c r="AO10" s="30">
+        <f t="shared" si="0"/>
+        <v>2.2333333333333334E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:41" x14ac:dyDescent="0.25">
+      <c r="B11" s="90" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="109"/>
+      <c r="D11" s="109"/>
+      <c r="E11" s="109"/>
+      <c r="F11" s="109"/>
+      <c r="G11" s="90"/>
+      <c r="H11" s="90">
+        <v>4.13</v>
+      </c>
+      <c r="I11" s="90"/>
+      <c r="J11" s="90"/>
+      <c r="K11" s="90"/>
+      <c r="L11" s="90">
+        <v>2E-3</v>
+      </c>
+      <c r="M11" s="90">
+        <v>0.70099999999999996</v>
+      </c>
+      <c r="N11" s="90">
+        <v>2.3E-2</v>
+      </c>
+      <c r="O11" s="90">
+        <v>6.2E-2</v>
+      </c>
+      <c r="P11" s="90">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="90">
+        <v>0</v>
+      </c>
+      <c r="R11" s="90">
+        <v>1E-3</v>
+      </c>
+      <c r="S11" s="22">
+        <v>1.9E-2</v>
+      </c>
+      <c r="T11" s="22">
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="U11" s="22">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="Z11" s="31"/>
+      <c r="AA11" s="31"/>
+      <c r="AB11" s="31">
+        <f t="shared" si="0"/>
+        <v>7.208333333333333</v>
+      </c>
+      <c r="AC11" s="31"/>
+      <c r="AD11" s="31"/>
+      <c r="AE11" s="31"/>
+      <c r="AF11" s="31">
+        <f t="shared" si="0"/>
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="AG11" s="31">
+        <f t="shared" si="0"/>
+        <v>0.39799999999999996</v>
+      </c>
+      <c r="AH11" s="31">
+        <f t="shared" si="0"/>
+        <v>0.33833333333333332</v>
+      </c>
+      <c r="AI11" s="31">
+        <f t="shared" si="0"/>
+        <v>4.3666666666666666E-2</v>
+      </c>
+      <c r="AJ11" s="31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AK11" s="31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AL11" s="31">
+        <f t="shared" si="0"/>
+        <v>3.0000000000000005E-3</v>
+      </c>
+      <c r="AM11" s="31">
+        <f t="shared" si="0"/>
+        <v>1.4333333333333332E-2</v>
+      </c>
+      <c r="AN11" s="31">
+        <f t="shared" si="0"/>
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="AO11" s="31">
+        <f t="shared" si="0"/>
+        <v>2.6666666666666668E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:41" x14ac:dyDescent="0.25">
+      <c r="B12" s="93" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="110"/>
+      <c r="D12" s="110"/>
+      <c r="E12" s="110"/>
+      <c r="F12" s="110"/>
+      <c r="G12" s="93"/>
+      <c r="H12" s="93">
+        <v>2.8340000000000001</v>
+      </c>
+      <c r="I12" s="93"/>
+      <c r="J12" s="93"/>
+      <c r="K12" s="93"/>
+      <c r="L12" s="93">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="M12" s="93">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="N12" s="93">
+        <v>0.112</v>
+      </c>
+      <c r="O12" s="93">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="P12" s="93">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="Q12" s="93">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="R12" s="93">
+        <v>0.185</v>
+      </c>
+      <c r="S12" s="18">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="T12" s="18">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="U12" s="18">
+        <v>0.15</v>
+      </c>
+      <c r="Z12" s="32"/>
+      <c r="AA12" s="32"/>
+      <c r="AB12" s="32">
+        <f t="shared" si="0"/>
+        <v>40.967333333333336</v>
+      </c>
+      <c r="AC12" s="32"/>
+      <c r="AD12" s="32"/>
+      <c r="AE12" s="32"/>
+      <c r="AF12" s="32">
+        <f t="shared" si="0"/>
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="AG12" s="32">
+        <f t="shared" si="0"/>
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="AH12" s="32">
+        <f t="shared" si="0"/>
+        <v>4.8999999999999995E-2</v>
+      </c>
+      <c r="AI12" s="32">
+        <f t="shared" si="0"/>
+        <v>1.6333333333333335E-2</v>
+      </c>
+      <c r="AJ12" s="32">
+        <f t="shared" si="0"/>
+        <v>7.6666666666666662E-3</v>
+      </c>
+      <c r="AK12" s="32">
+        <f t="shared" si="0"/>
+        <v>1.6666666666666668E-3</v>
+      </c>
+      <c r="AL12" s="32">
+        <f t="shared" si="0"/>
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="AM12" s="32">
+        <f t="shared" si="0"/>
+        <v>0.23433333333333331</v>
+      </c>
+      <c r="AN12" s="32">
+        <f t="shared" si="0"/>
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="AO12" s="32">
+        <f t="shared" si="0"/>
+        <v>0.22833333333333336</v>
+      </c>
+    </row>
+    <row r="13" spans="2:41" x14ac:dyDescent="0.25">
+      <c r="B13" s="140" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="140"/>
+      <c r="D13" s="140"/>
+      <c r="E13" s="140"/>
+      <c r="F13" s="140"/>
+      <c r="G13" s="140"/>
+      <c r="H13" s="140">
+        <v>4.1340000000000003</v>
+      </c>
+      <c r="I13" s="140"/>
+      <c r="J13" s="140"/>
+      <c r="K13" s="140"/>
+      <c r="L13" s="140">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="M13" s="140">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="N13" s="140">
+        <v>0</v>
+      </c>
+      <c r="O13" s="140">
+        <v>0.40300000000000002</v>
+      </c>
+      <c r="P13" s="140">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="140">
+        <v>0</v>
+      </c>
+      <c r="R13" s="140">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="S13" s="140">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="T13" s="140">
+        <v>1.9E-2</v>
+      </c>
+      <c r="U13" s="140">
+        <v>0.38500000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="2:41" x14ac:dyDescent="0.25">
+      <c r="B14" s="114" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4">
+        <f>AVERAGE(H4:H13)</f>
+        <v>5.8619000000000003</v>
+      </c>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4">
+        <f t="shared" ref="I14:U14" si="1">AVERAGE(L4:L13)</f>
+        <v>0.1169</v>
+      </c>
+      <c r="M14" s="4">
+        <f t="shared" si="1"/>
+        <v>0.14189999999999997</v>
+      </c>
+      <c r="N14" s="4">
+        <f t="shared" si="1"/>
+        <v>0.10870000000000002</v>
+      </c>
+      <c r="O14" s="4">
+        <f t="shared" si="1"/>
+        <v>0.23630000000000001</v>
+      </c>
+      <c r="P14" s="4">
+        <f t="shared" si="1"/>
+        <v>2.1999999999999997E-3</v>
+      </c>
+      <c r="Q14" s="4">
+        <f t="shared" si="1"/>
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="R14" s="4">
+        <f t="shared" si="1"/>
+        <v>2.9099999999999997E-2</v>
+      </c>
+      <c r="S14" s="4">
+        <f t="shared" si="1"/>
+        <v>0.13250000000000001</v>
+      </c>
+      <c r="T14" s="4">
+        <f t="shared" si="1"/>
+        <v>6.2399999999999997E-2</v>
+      </c>
+      <c r="U14" s="4">
+        <f t="shared" si="1"/>
+        <v>0.1691</v>
+      </c>
+    </row>
+    <row r="15" spans="2:41" x14ac:dyDescent="0.25">
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="2:41" x14ac:dyDescent="0.25">
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B17" s="136" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="136"/>
+      <c r="D17" s="136"/>
+      <c r="E17" s="136"/>
+      <c r="F17" s="136"/>
+      <c r="G17" s="136"/>
+      <c r="H17" s="136"/>
+      <c r="I17" s="136"/>
+      <c r="J17" s="136"/>
+      <c r="K17" s="136"/>
+      <c r="L17" s="136"/>
+      <c r="M17" s="136"/>
+      <c r="N17" s="136"/>
+      <c r="O17" s="136"/>
+      <c r="P17" s="136"/>
+      <c r="Q17" s="136"/>
+      <c r="R17" s="136"/>
+      <c r="S17" s="136" t="s">
+        <v>28</v>
+      </c>
+      <c r="T17" s="136"/>
+      <c r="U17" s="136"/>
+      <c r="V17" s="136"/>
+      <c r="W17" s="136"/>
+      <c r="X17" s="136"/>
+      <c r="Y17" s="136"/>
+      <c r="Z17" s="136"/>
+      <c r="AA17" s="136"/>
+      <c r="AB17" s="136"/>
+      <c r="AC17" s="136"/>
+      <c r="AD17" s="136"/>
+      <c r="AE17" s="136"/>
+      <c r="AF17" s="136"/>
+      <c r="AG17" s="136"/>
+      <c r="AH17" s="136"/>
+      <c r="AI17" s="136"/>
+    </row>
+    <row r="18" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B18" s="99" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="126" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="127" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="127" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="127" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" s="127" t="s">
+        <v>15</v>
+      </c>
+      <c r="H18" s="127" t="s">
+        <v>14</v>
+      </c>
+      <c r="I18" s="127" t="s">
+        <v>16</v>
+      </c>
+      <c r="J18" s="127" t="s">
+        <v>29</v>
+      </c>
+      <c r="K18" s="128" t="s">
+        <v>17</v>
+      </c>
+      <c r="L18" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="M18" s="127"/>
+      <c r="N18" s="127"/>
+      <c r="O18" s="127"/>
+      <c r="P18" s="127"/>
+      <c r="Q18" s="127"/>
+      <c r="R18" s="127"/>
+      <c r="S18" s="127"/>
+      <c r="T18" s="127"/>
+      <c r="U18" s="128"/>
+    </row>
+    <row r="19" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B19" s="100"/>
+      <c r="C19" s="130"/>
+      <c r="D19" s="124"/>
+      <c r="E19" s="124"/>
+      <c r="F19" s="124"/>
+      <c r="G19" s="124"/>
+      <c r="H19" s="124"/>
+      <c r="I19" s="124"/>
+      <c r="J19" s="124"/>
+      <c r="K19" s="125"/>
+      <c r="L19" s="111" t="s">
+        <v>18</v>
+      </c>
+      <c r="M19" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="N19" s="56" t="s">
+        <v>20</v>
+      </c>
+      <c r="O19" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="P19" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q19" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="R19" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="S19" s="112" t="s">
+        <v>39</v>
+      </c>
+      <c r="T19" s="112" t="s">
+        <v>40</v>
+      </c>
+      <c r="U19" s="113" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B20" s="101" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="102"/>
+      <c r="D20" s="102"/>
+      <c r="E20" s="102"/>
+      <c r="F20" s="101"/>
+      <c r="G20" s="101"/>
+      <c r="H20" s="101">
+        <v>13.295999999999999</v>
+      </c>
+      <c r="I20" s="101"/>
+      <c r="J20" s="101"/>
+      <c r="K20" s="101"/>
+      <c r="L20" s="101">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="M20" s="101">
+        <v>1E-3</v>
+      </c>
+      <c r="N20" s="101">
+        <v>1E-3</v>
+      </c>
+      <c r="O20" s="101">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="P20" s="101">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="101">
+        <v>0</v>
+      </c>
+      <c r="R20" s="101">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="S20" s="6">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="T20" s="6">
+        <v>0.89300000000000002</v>
+      </c>
+      <c r="U20" s="6">
+        <v>1.4E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B21" s="72" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="103"/>
+      <c r="D21" s="103"/>
+      <c r="E21" s="103"/>
+      <c r="F21" s="103"/>
+      <c r="G21" s="72"/>
+      <c r="H21" s="72">
+        <v>12.439</v>
+      </c>
+      <c r="I21" s="72"/>
+      <c r="J21" s="72"/>
+      <c r="K21" s="72"/>
+      <c r="L21" s="72">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="M21" s="72">
+        <v>0.36199999999999999</v>
+      </c>
+      <c r="N21" s="72">
+        <v>0.46400000000000002</v>
+      </c>
+      <c r="O21" s="72">
+        <v>0.36199999999999999</v>
+      </c>
+      <c r="P21" s="72">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="72">
+        <v>0</v>
+      </c>
+      <c r="R21" s="72">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="S21" s="8">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="T21" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="U21" s="8">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B22" s="75" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="104"/>
+      <c r="D22" s="104"/>
+      <c r="E22" s="104"/>
+      <c r="F22" s="104"/>
+      <c r="G22" s="75"/>
+      <c r="H22" s="75">
+        <v>5.5170000000000003</v>
+      </c>
+      <c r="I22" s="75"/>
+      <c r="J22" s="75"/>
+      <c r="K22" s="75"/>
+      <c r="L22" s="75">
+        <v>0.193</v>
+      </c>
+      <c r="M22" s="75">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="N22" s="75">
+        <v>0</v>
+      </c>
+      <c r="O22" s="75">
+        <v>6.3E-2</v>
+      </c>
+      <c r="P22" s="75">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="75">
+        <v>2E-3</v>
+      </c>
+      <c r="R22" s="75">
+        <v>0.121</v>
+      </c>
+      <c r="S22" s="10">
+        <v>0.254</v>
+      </c>
+      <c r="T22" s="10">
+        <v>0.125</v>
+      </c>
+      <c r="U22" s="10">
+        <v>0.23499999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B23" s="78" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="105"/>
+      <c r="D23" s="105"/>
+      <c r="E23" s="105"/>
+      <c r="F23" s="105"/>
+      <c r="G23" s="78"/>
+      <c r="H23" s="78">
+        <v>7.3049999999999997</v>
+      </c>
+      <c r="I23" s="78"/>
+      <c r="J23" s="78"/>
+      <c r="K23" s="78"/>
+      <c r="L23" s="78">
+        <v>2.7E-2</v>
+      </c>
+      <c r="M23" s="78">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="N23" s="78">
+        <v>0.157</v>
+      </c>
+      <c r="O23" s="78">
+        <v>0.34200000000000003</v>
+      </c>
+      <c r="P23" s="78">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="78">
+        <v>0</v>
+      </c>
+      <c r="R23" s="78">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="S23" s="12">
+        <v>0</v>
+      </c>
+      <c r="T23" s="12">
+        <v>0</v>
+      </c>
+      <c r="U23" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B24" s="81" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="106"/>
+      <c r="D24" s="106"/>
+      <c r="E24" s="106"/>
+      <c r="F24" s="106"/>
+      <c r="G24" s="81"/>
+      <c r="H24" s="81">
+        <v>1.175</v>
+      </c>
+      <c r="I24" s="81"/>
+      <c r="J24" s="81"/>
+      <c r="K24" s="81"/>
+      <c r="L24" s="81">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="M24" s="81">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="N24" s="81">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="O24" s="81">
+        <v>0.79400000000000004</v>
+      </c>
+      <c r="P24" s="81">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="81">
+        <v>1E-3</v>
+      </c>
+      <c r="R24" s="81">
+        <v>1E-3</v>
+      </c>
+      <c r="S24" s="20">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="T24" s="20">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="U24" s="20">
+        <v>5.1999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B25" s="84" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="107"/>
+      <c r="D25" s="107"/>
+      <c r="E25" s="107"/>
+      <c r="F25" s="107"/>
+      <c r="G25" s="84"/>
+      <c r="H25" s="84">
+        <v>7.9630000000000001</v>
+      </c>
+      <c r="I25" s="84"/>
+      <c r="J25" s="84"/>
+      <c r="K25" s="84"/>
+      <c r="L25" s="84">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="M25" s="84">
+        <v>0.73699999999999999</v>
+      </c>
+      <c r="N25" s="84">
+        <v>1E-3</v>
+      </c>
+      <c r="O25" s="84">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="P25" s="84">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="84">
+        <v>0</v>
+      </c>
+      <c r="R25" s="84">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="S25" s="16">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="T25" s="16">
+        <v>1.2E-2</v>
+      </c>
+      <c r="U25" s="16">
+        <v>7.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B26" s="87" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" s="108"/>
+      <c r="D26" s="108"/>
+      <c r="E26" s="108"/>
+      <c r="F26" s="108"/>
+      <c r="G26" s="87"/>
+      <c r="H26" s="87">
+        <v>13.478999999999999</v>
+      </c>
+      <c r="I26" s="87"/>
+      <c r="J26" s="87"/>
+      <c r="K26" s="87"/>
+      <c r="L26" s="87">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="M26" s="87">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="N26" s="87">
+        <v>0.41199999999999998</v>
+      </c>
+      <c r="O26" s="87">
+        <v>0</v>
+      </c>
+      <c r="P26" s="87">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="87">
+        <v>0</v>
+      </c>
+      <c r="R26" s="87">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="S26" s="14">
+        <v>0.04</v>
+      </c>
+      <c r="T26" s="14">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="U26" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="W26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B27" s="90" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="109"/>
+      <c r="D27" s="109"/>
+      <c r="E27" s="109"/>
+      <c r="F27" s="109"/>
+      <c r="G27" s="90"/>
+      <c r="H27" s="90">
+        <v>10.212</v>
+      </c>
+      <c r="I27" s="90"/>
+      <c r="J27" s="90"/>
+      <c r="K27" s="90"/>
+      <c r="L27" s="90">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="M27" s="90">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="N27" s="90">
+        <v>0.84199999999999997</v>
+      </c>
+      <c r="O27" s="90">
+        <v>0</v>
+      </c>
+      <c r="P27" s="90">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="90">
+        <v>0</v>
+      </c>
+      <c r="R27" s="90">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="S27" s="22">
+        <v>1E-3</v>
+      </c>
+      <c r="T27" s="22">
+        <v>1E-3</v>
+      </c>
+      <c r="U27" s="22">
+        <v>2E-3</v>
+      </c>
+      <c r="W27" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B28" s="93" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" s="110"/>
+      <c r="D28" s="110"/>
+      <c r="E28" s="110"/>
+      <c r="F28" s="110"/>
+      <c r="G28" s="93"/>
+      <c r="H28" s="93">
+        <v>55.436</v>
+      </c>
+      <c r="I28" s="93"/>
+      <c r="J28" s="93"/>
+      <c r="K28" s="93"/>
+      <c r="L28" s="93">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="M28" s="93">
+        <v>0.106</v>
+      </c>
+      <c r="N28" s="93">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="O28" s="93">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="P28" s="93">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="93">
+        <v>0</v>
+      </c>
+      <c r="R28" s="93">
+        <v>0.157</v>
+      </c>
+      <c r="S28" s="18">
+        <v>0.254</v>
+      </c>
+      <c r="T28" s="18">
+        <v>0.124</v>
+      </c>
+      <c r="U28" s="18">
+        <v>0.22</v>
+      </c>
+      <c r="W28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B29" s="140" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29" s="140"/>
+      <c r="D29" s="140"/>
+      <c r="E29" s="140"/>
+      <c r="F29" s="140"/>
+      <c r="G29" s="140"/>
+      <c r="H29" s="140">
+        <v>5.351</v>
+      </c>
+      <c r="I29" s="140"/>
+      <c r="J29" s="140"/>
+      <c r="K29" s="140"/>
+      <c r="L29" s="140">
+        <v>0.19</v>
+      </c>
+      <c r="M29" s="140">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="N29" s="140">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="O29" s="140">
+        <v>0.187</v>
+      </c>
+      <c r="P29" s="140">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="140">
+        <v>0</v>
+      </c>
+      <c r="R29" s="140">
+        <v>0.08</v>
+      </c>
+      <c r="S29" s="140">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="T29" s="140">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="U29" s="140">
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="W29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B30" s="114" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4">
+        <f>AVERAGE(H20:H29)</f>
+        <v>13.2173</v>
+      </c>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4">
+        <f t="shared" ref="I30:U30" si="2">AVERAGE(L20:L29)</f>
+        <v>7.8300000000000008E-2</v>
+      </c>
+      <c r="M30" s="4">
+        <f t="shared" si="2"/>
+        <v>0.22399999999999998</v>
+      </c>
+      <c r="N30" s="4">
+        <f t="shared" si="2"/>
+        <v>0.20099999999999998</v>
+      </c>
+      <c r="O30" s="4">
+        <f t="shared" si="2"/>
+        <v>0.1971</v>
+      </c>
+      <c r="P30" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q30" s="4">
+        <f t="shared" si="2"/>
+        <v>3.0000000000000003E-4</v>
+      </c>
+      <c r="R30" s="4">
+        <f t="shared" si="2"/>
+        <v>3.8600000000000009E-2</v>
+      </c>
+      <c r="S30" s="4">
+        <f t="shared" si="2"/>
+        <v>8.14E-2</v>
+      </c>
+      <c r="T30" s="4">
+        <f t="shared" si="2"/>
+        <v>0.13329999999999997</v>
+      </c>
+      <c r="U30" s="4">
+        <f t="shared" si="2"/>
+        <v>7.0099999999999996E-2</v>
+      </c>
+      <c r="W30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="W31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="W32" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B33" s="136" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33" s="136"/>
+      <c r="D33" s="136"/>
+      <c r="E33" s="136"/>
+      <c r="F33" s="136"/>
+      <c r="G33" s="136"/>
+      <c r="H33" s="136"/>
+      <c r="I33" s="136"/>
+      <c r="J33" s="136"/>
+      <c r="K33" s="136"/>
+      <c r="L33" s="136"/>
+      <c r="M33" s="136"/>
+      <c r="N33" s="136"/>
+      <c r="O33" s="136"/>
+      <c r="P33" s="136"/>
+      <c r="Q33" s="136"/>
+      <c r="R33" s="136"/>
+    </row>
+    <row r="34" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B34" s="99" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" s="126" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34" s="127" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" s="127" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" s="127" t="s">
+        <v>13</v>
+      </c>
+      <c r="G34" s="127" t="s">
+        <v>15</v>
+      </c>
+      <c r="H34" s="127" t="s">
+        <v>14</v>
+      </c>
+      <c r="I34" s="127" t="s">
+        <v>16</v>
+      </c>
+      <c r="J34" s="127" t="s">
+        <v>29</v>
+      </c>
+      <c r="K34" s="128" t="s">
+        <v>17</v>
+      </c>
+      <c r="L34" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="M34" s="127"/>
+      <c r="N34" s="127"/>
+      <c r="O34" s="127"/>
+      <c r="P34" s="127"/>
+      <c r="Q34" s="127"/>
+      <c r="R34" s="127"/>
+      <c r="S34" s="127"/>
+      <c r="T34" s="127"/>
+      <c r="U34" s="128"/>
+    </row>
+    <row r="35" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B35" s="100"/>
+      <c r="C35" s="130"/>
+      <c r="D35" s="124"/>
+      <c r="E35" s="124"/>
+      <c r="F35" s="124"/>
+      <c r="G35" s="124"/>
+      <c r="H35" s="124"/>
+      <c r="I35" s="124"/>
+      <c r="J35" s="124"/>
+      <c r="K35" s="125"/>
+      <c r="L35" s="111" t="s">
+        <v>18</v>
+      </c>
+      <c r="M35" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="N35" s="56" t="s">
+        <v>20</v>
+      </c>
+      <c r="O35" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="P35" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q35" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="R35" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="S35" s="112" t="s">
+        <v>39</v>
+      </c>
+      <c r="T35" s="112" t="s">
+        <v>40</v>
+      </c>
+      <c r="U35" s="113" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B36" s="101" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" s="115"/>
+      <c r="D36" s="115"/>
+      <c r="E36" s="115"/>
+      <c r="F36" s="115"/>
+      <c r="G36" s="115"/>
+      <c r="H36" s="115">
+        <v>27.047999999999998</v>
+      </c>
+      <c r="I36" s="115"/>
+      <c r="J36" s="115"/>
+      <c r="K36" s="116"/>
+      <c r="L36" s="116">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="M36" s="116">
+        <v>0</v>
+      </c>
+      <c r="N36" s="116">
+        <v>1E-3</v>
+      </c>
+      <c r="O36" s="116">
+        <v>0.104</v>
+      </c>
+      <c r="P36" s="116">
+        <v>0</v>
+      </c>
+      <c r="Q36" s="120">
+        <v>0</v>
+      </c>
+      <c r="R36" s="120">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="S36" s="121">
+        <v>0.156</v>
+      </c>
+      <c r="T36" s="121">
+        <v>0.32700000000000001</v>
+      </c>
+      <c r="U36" s="121">
+        <v>0.161</v>
+      </c>
+    </row>
+    <row r="37" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B37" s="72" t="s">
+        <v>1</v>
+      </c>
+      <c r="C37" s="103"/>
+      <c r="D37" s="103"/>
+      <c r="E37" s="103"/>
+      <c r="F37" s="103"/>
+      <c r="G37" s="72"/>
+      <c r="H37" s="72">
+        <v>12.36</v>
+      </c>
+      <c r="I37" s="72"/>
+      <c r="J37" s="72"/>
+      <c r="K37" s="72"/>
+      <c r="L37" s="72">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="M37" s="72">
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="N37" s="72">
+        <v>0.45300000000000001</v>
+      </c>
+      <c r="O37" s="72">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="P37" s="72">
+        <v>0</v>
+      </c>
+      <c r="Q37" s="72">
+        <v>0</v>
+      </c>
+      <c r="R37" s="72">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="S37" s="8">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="T37" s="8">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="U37" s="8">
+        <v>3.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B38" s="75" t="s">
+        <v>2</v>
+      </c>
+      <c r="C38" s="104"/>
+      <c r="D38" s="104"/>
+      <c r="E38" s="104"/>
+      <c r="F38" s="104"/>
+      <c r="G38" s="75"/>
+      <c r="H38" s="75">
+        <v>10.967000000000001</v>
+      </c>
+      <c r="I38" s="75"/>
+      <c r="J38" s="75"/>
+      <c r="K38" s="75"/>
+      <c r="L38" s="75">
+        <v>4.7E-2</v>
+      </c>
+      <c r="M38" s="75">
+        <v>0</v>
+      </c>
+      <c r="N38" s="75">
+        <v>0</v>
+      </c>
+      <c r="O38" s="75">
+        <v>0.85899999999999999</v>
+      </c>
+      <c r="P38" s="75">
+        <v>0</v>
+      </c>
+      <c r="Q38" s="75">
+        <v>0</v>
+      </c>
+      <c r="R38" s="75">
+        <v>0.02</v>
+      </c>
+      <c r="S38" s="10">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="T38" s="10">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="U38" s="10">
+        <v>3.2000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B39" s="78" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39" s="105"/>
+      <c r="D39" s="105"/>
+      <c r="E39" s="105"/>
+      <c r="F39" s="105"/>
+      <c r="G39" s="78"/>
+      <c r="H39" s="78">
+        <v>24.571999999999999</v>
+      </c>
+      <c r="I39" s="78"/>
+      <c r="J39" s="78"/>
+      <c r="K39" s="78"/>
+      <c r="L39" s="78">
+        <v>0.15</v>
+      </c>
+      <c r="M39" s="78">
+        <v>0.57899999999999996</v>
+      </c>
+      <c r="N39" s="78">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="O39" s="78">
+        <v>1.9E-2</v>
+      </c>
+      <c r="P39" s="78">
+        <v>0</v>
+      </c>
+      <c r="Q39" s="78">
+        <v>0</v>
+      </c>
+      <c r="R39" s="78">
+        <v>0.22600000000000001</v>
+      </c>
+      <c r="S39" s="12">
+        <v>0</v>
+      </c>
+      <c r="T39" s="12">
+        <v>0</v>
+      </c>
+      <c r="U39" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B40" s="81" t="s">
+        <v>4</v>
+      </c>
+      <c r="C40" s="106"/>
+      <c r="D40" s="106"/>
+      <c r="E40" s="106"/>
+      <c r="F40" s="106"/>
+      <c r="G40" s="81"/>
+      <c r="H40" s="81">
+        <v>3.9239999999999999</v>
+      </c>
+      <c r="I40" s="81"/>
+      <c r="J40" s="81"/>
+      <c r="K40" s="81"/>
+      <c r="L40" s="81">
+        <v>0</v>
+      </c>
+      <c r="M40" s="81">
+        <v>0.99199999999999999</v>
+      </c>
+      <c r="N40" s="81">
+        <v>1E-3</v>
+      </c>
+      <c r="O40" s="81">
+        <v>1E-3</v>
+      </c>
+      <c r="P40" s="81">
+        <v>0</v>
+      </c>
+      <c r="Q40" s="81">
+        <v>0</v>
+      </c>
+      <c r="R40" s="81">
+        <v>0</v>
+      </c>
+      <c r="S40" s="20">
+        <v>2E-3</v>
+      </c>
+      <c r="T40" s="20">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="U40" s="20">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B41" s="84" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" s="107"/>
+      <c r="D41" s="107"/>
+      <c r="E41" s="107"/>
+      <c r="F41" s="107"/>
+      <c r="G41" s="84"/>
+      <c r="H41" s="84">
+        <v>2.4289999999999998</v>
+      </c>
+      <c r="I41" s="84"/>
+      <c r="J41" s="84"/>
+      <c r="K41" s="84"/>
+      <c r="L41" s="84">
+        <v>1E-3</v>
+      </c>
+      <c r="M41" s="84">
+        <v>0.25900000000000001</v>
+      </c>
+      <c r="N41" s="84">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="O41" s="84">
+        <v>0.46300000000000002</v>
+      </c>
+      <c r="P41" s="84">
+        <v>0</v>
+      </c>
+      <c r="Q41" s="84">
+        <v>0</v>
+      </c>
+      <c r="R41" s="84">
+        <v>1E-3</v>
+      </c>
+      <c r="S41" s="16">
+        <v>0.153</v>
+      </c>
+      <c r="T41" s="16">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="U41" s="16">
+        <v>7.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B42" s="87" t="s">
+        <v>6</v>
+      </c>
+      <c r="C42" s="108"/>
+      <c r="D42" s="108"/>
+      <c r="E42" s="108"/>
+      <c r="F42" s="108"/>
+      <c r="G42" s="87"/>
+      <c r="H42" s="87">
+        <v>0.43</v>
+      </c>
+      <c r="I42" s="87"/>
+      <c r="J42" s="87"/>
+      <c r="K42" s="87"/>
+      <c r="L42" s="87">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="M42" s="87">
+        <v>0</v>
+      </c>
+      <c r="N42" s="87">
+        <v>0</v>
+      </c>
+      <c r="O42" s="87">
+        <v>0.95299999999999996</v>
+      </c>
+      <c r="P42" s="87">
+        <v>0</v>
+      </c>
+      <c r="Q42" s="87">
+        <v>0</v>
+      </c>
+      <c r="R42" s="87">
+        <v>2E-3</v>
+      </c>
+      <c r="S42" s="14">
+        <v>1.9E-2</v>
+      </c>
+      <c r="T42" s="14">
+        <v>2E-3</v>
+      </c>
+      <c r="U42" s="14">
+        <v>1.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B43" s="90" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43" s="109"/>
+      <c r="D43" s="109"/>
+      <c r="E43" s="109"/>
+      <c r="F43" s="109"/>
+      <c r="G43" s="90"/>
+      <c r="H43" s="90">
+        <v>7.2830000000000004</v>
+      </c>
+      <c r="I43" s="90"/>
+      <c r="J43" s="90"/>
+      <c r="K43" s="90"/>
+      <c r="L43" s="90">
+        <v>1.6E-2</v>
+      </c>
+      <c r="M43" s="90">
+        <v>0.35099999999999998</v>
+      </c>
+      <c r="N43" s="90">
+        <v>0.15</v>
+      </c>
+      <c r="O43" s="90">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="P43" s="90">
+        <v>0</v>
+      </c>
+      <c r="Q43" s="90">
+        <v>0</v>
+      </c>
+      <c r="R43" s="90">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="S43" s="22">
+        <v>2.3E-2</v>
+      </c>
+      <c r="T43" s="22">
+        <v>0.38100000000000001</v>
+      </c>
+      <c r="U43" s="22">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B44" s="93" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" s="110"/>
+      <c r="D44" s="110"/>
+      <c r="E44" s="110"/>
+      <c r="F44" s="110"/>
+      <c r="G44" s="93"/>
+      <c r="H44" s="93">
+        <v>64.632000000000005</v>
+      </c>
+      <c r="I44" s="93"/>
+      <c r="J44" s="93"/>
+      <c r="K44" s="93"/>
+      <c r="L44" s="93">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="M44" s="93">
+        <v>2E-3</v>
+      </c>
+      <c r="N44" s="93">
+        <v>2.7E-2</v>
+      </c>
+      <c r="O44" s="93">
+        <v>1E-3</v>
+      </c>
+      <c r="P44" s="93">
+        <v>1E-3</v>
+      </c>
+      <c r="Q44" s="93">
+        <v>0</v>
+      </c>
+      <c r="R44" s="93">
+        <v>0.159</v>
+      </c>
+      <c r="S44" s="18">
+        <v>0.214</v>
+      </c>
+      <c r="T44" s="18">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="U44" s="18">
+        <v>0.315</v>
+      </c>
+    </row>
+    <row r="45" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B45" s="140" t="s">
+        <v>42</v>
+      </c>
+      <c r="C45" s="140"/>
+      <c r="D45" s="140"/>
+      <c r="E45" s="140"/>
+      <c r="F45" s="140"/>
+      <c r="G45" s="140"/>
+      <c r="H45" s="140">
+        <v>13.093</v>
+      </c>
+      <c r="I45" s="140"/>
+      <c r="J45" s="140"/>
+      <c r="K45" s="140"/>
+      <c r="L45" s="140">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="M45" s="140">
+        <v>1E-3</v>
+      </c>
+      <c r="N45" s="140">
+        <v>0</v>
+      </c>
+      <c r="O45" s="140">
+        <v>0.81599999999999995</v>
+      </c>
+      <c r="P45" s="140">
+        <v>0</v>
+      </c>
+      <c r="Q45" s="140">
+        <v>0</v>
+      </c>
+      <c r="R45" s="140">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="S45" s="140">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="T45" s="140">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="U45" s="140">
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B46" s="114" t="s">
+        <v>33</v>
+      </c>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
+      <c r="H46" s="4">
+        <f>AVERAGE(H36:H45)</f>
+        <v>16.673800000000004</v>
+      </c>
+      <c r="I46" s="4"/>
+      <c r="J46" s="4"/>
+      <c r="K46" s="4"/>
+      <c r="L46" s="4">
+        <f t="shared" ref="I46:U46" si="3">AVERAGE(L36:L45)</f>
+        <v>6.3899999999999998E-2</v>
+      </c>
+      <c r="M46" s="4">
+        <f t="shared" si="3"/>
+        <v>0.24599999999999994</v>
+      </c>
+      <c r="N46" s="4">
+        <f t="shared" si="3"/>
+        <v>6.6299999999999998E-2</v>
+      </c>
+      <c r="O46" s="4">
+        <f t="shared" si="3"/>
+        <v>0.33199999999999996</v>
+      </c>
+      <c r="P46" s="4">
+        <f t="shared" si="3"/>
+        <v>1E-4</v>
+      </c>
+      <c r="Q46" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="R46" s="4">
+        <f t="shared" si="3"/>
+        <v>5.2200000000000003E-2</v>
+      </c>
+      <c r="S46" s="4">
+        <f t="shared" si="3"/>
+        <v>7.2600000000000012E-2</v>
+      </c>
+      <c r="T46" s="4">
+        <f t="shared" si="3"/>
+        <v>0.1066</v>
+      </c>
+      <c r="U46" s="4">
+        <f t="shared" si="3"/>
+        <v>5.9299999999999999E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="42">
+    <mergeCell ref="I34:I35"/>
+    <mergeCell ref="J34:J35"/>
+    <mergeCell ref="K34:K35"/>
+    <mergeCell ref="L34:U34"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="G34:G35"/>
+    <mergeCell ref="H34:H35"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="J18:J19"/>
+    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="L18:U18"/>
+    <mergeCell ref="B33:R33"/>
+    <mergeCell ref="AD2:AD3"/>
+    <mergeCell ref="AE2:AE3"/>
+    <mergeCell ref="AF2:AO2"/>
+    <mergeCell ref="B17:R17"/>
+    <mergeCell ref="S17:AI17"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="L2:U2"/>
+    <mergeCell ref="Z2:Z3"/>
+    <mergeCell ref="AA2:AA3"/>
+    <mergeCell ref="AB2:AB3"/>
+    <mergeCell ref="AC2:AC3"/>
+    <mergeCell ref="B1:R1"/>
+    <mergeCell ref="Z1:AE1"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:J3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>